<commit_message>
Práctica Tabla de Frecuencias
Se termina la práctica Tabla de Frecuencias para la guía com para los profesores
</commit_message>
<xml_diff>
--- a/10_Practicas/Tabla_de_Frecuencias/Ejemplo/Resultados/Resultados_Ej_Temp_Ad.xlsx
+++ b/10_Practicas/Tabla_de_Frecuencias/Ejemplo/Resultados/Resultados_Ej_Temp_Ad.xlsx
@@ -50,25 +50,25 @@
     <t>FRA</t>
   </si>
   <si>
-    <t>(38.79, 47.34)</t>
-  </si>
-  <si>
-    <t>(47.34, 55.89)</t>
-  </si>
-  <si>
-    <t>(55.89, 64.43)</t>
-  </si>
-  <si>
-    <t>(64.43, 72.98)</t>
-  </si>
-  <si>
-    <t>(72.98, 81.52)</t>
-  </si>
-  <si>
-    <t>(81.52, 90.07)</t>
-  </si>
-  <si>
-    <t>(90.07, 98.61)</t>
+    <t>[38.0, 44.0]</t>
+  </si>
+  <si>
+    <t>[44.0, 50.0]</t>
+  </si>
+  <si>
+    <t>[50.0, 56.0]</t>
+  </si>
+  <si>
+    <t>[56.0, 62.0]</t>
+  </si>
+  <si>
+    <t>[62.0, 68.0]</t>
+  </si>
+  <si>
+    <t>[68.0, 74.0]</t>
+  </si>
+  <si>
+    <t>[74.0, 80.0]</t>
   </si>
   <si>
     <t>Medidas De Centramiento Y Dispersión</t>
@@ -465,7 +465,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>69.67333333333333</v>
+        <v>59.73125</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -473,7 +473,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>69.8</v>
+        <v>59.6</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -481,7 +481,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>66</v>
+        <v>65.5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -489,7 +489,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>10.01108898384981</v>
+        <v>7.274145622753864</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -497,7 +497,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>59.8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -505,7 +505,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1">
-        <v>100.2219026425591</v>
+        <v>52.91319454102921</v>
       </c>
     </row>
   </sheetData>
@@ -521,7 +521,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
   </cols>
@@ -587,16 +587,16 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C6" s="1">
-        <v>0.2277777777777778</v>
+        <v>0.2263888888888889</v>
       </c>
       <c r="D6">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E6" s="1">
-        <v>0.3055555555555556</v>
+        <v>0.3041666666666666</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -604,16 +604,16 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C7" s="1">
-        <v>0.3236111111111111</v>
+        <v>0.3222222222222222</v>
       </c>
       <c r="D7">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E7" s="1">
-        <v>0.6291666666666667</v>
+        <v>0.6263888888888889</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -621,10 +621,10 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C8" s="1">
-        <v>0.25</v>
+        <v>0.2527777777777778</v>
       </c>
       <c r="D8">
         <v>633</v>
@@ -638,16 +638,16 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="1">
-        <v>0.1</v>
+        <v>0.09861111111111111</v>
       </c>
       <c r="D9">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E9" s="1">
-        <v>0.9791666666666666</v>
+        <v>0.9777777777777777</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -655,10 +655,10 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1">
-        <v>0.02083333333333333</v>
+        <v>0.02222222222222222</v>
       </c>
       <c r="D10">
         <v>720</v>

</xml_diff>